<commit_message>
update JDT and add figma link for maquette
</commit_message>
<xml_diff>
--- a/JDT/cdUHYdbfWxdDjDBrdTIEeiEltL7VAmjO9XU2JjvP.xlsx
+++ b/JDT/cdUHYdbfWxdDjDBrdTIEeiEltL7VAmjO9XU2JjvP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu41ecx\Documents\GitHub\P-AppMobile\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227AC0A0-5F39-4004-A980-2B02652C9371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4BB879-2426-4CA2-92F7-F258DCB6C538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -120,13 +120,22 @@
     <t>Autre</t>
   </si>
   <si>
-    <t>Nom Prénom</t>
-  </si>
-  <si>
     <t>18.03.2024  au 27.05.2024</t>
   </si>
   <si>
     <t>P_App - 335 - Passion Lecture</t>
+  </si>
+  <si>
+    <t>Présentation du projet, inscription sur le marcket place et mise en place des fichiers de projet</t>
+  </si>
+  <si>
+    <t>Alessio Lopardo</t>
+  </si>
+  <si>
+    <t>Lecture du cahier des charge et du document sur le stockage de données en binaire MySQL BLOB</t>
+  </si>
+  <si>
+    <t>Maquette de l'application mobile sur figma</t>
   </si>
 </sst>
 </file>
@@ -1024,16 +1033,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1949,7 +1958,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1985,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="53" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" s="53"/>
       <c r="E2" s="53"/>
@@ -1993,7 +2002,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -2002,7 +2011,7 @@
       </c>
       <c r="C3" s="24" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 0 minutes</v>
+        <v>0 jours 2 heurs 45 minutes</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -2010,22 +2019,22 @@
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="23.25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="24">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="24">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="E4" s="51">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2068,20 +2077,35 @@
         <v>45369</v>
       </c>
       <c r="C7" s="33"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="47"/>
+      <c r="D7" s="41">
+        <v>45</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="str">
+      <c r="A8" s="8">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="38"/>
+        <v>12</v>
+      </c>
+      <c r="B8" s="38">
+        <v>45369</v>
+      </c>
       <c r="C8" s="34"/>
-      <c r="D8" s="42"/>
-      <c r="F8" s="47"/>
+      <c r="D8" s="42">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="17"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -2094,15 +2118,25 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="str">
+      <c r="A9" s="8">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="47"/>
+        <v>12</v>
+      </c>
+      <c r="B9" s="39">
+        <v>45369</v>
+      </c>
+      <c r="C9" s="35">
+        <v>1</v>
+      </c>
+      <c r="D9" s="43">
+        <v>30</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="19"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -8337,7 +8371,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8345,7 +8379,7 @@
       </c>
       <c r="D7" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8355,7 +8389,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C8" s="30" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8363,7 +8397,7 @@
       </c>
       <c r="D8" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -8387,7 +8421,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C10" s="48" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8395,7 +8429,7 @@
       </c>
       <c r="D10" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8418,7 +8452,7 @@
       </c>
       <c r="D12" s="45">
         <f>SUM(D4:D11)</f>
-        <v>0</v>
+        <v>7.2916666666666657E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8697,6 +8731,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8706,15 +8749,6 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8738,6 +8772,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8749,12 +8791,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>